<commit_message>
Starting item and inventory system + nearly finished tests for item containers, possibly turn Item scripts into humble objects to make testing easier
</commit_message>
<xml_diff>
--- a/Scheduling.xlsx
+++ b/Scheduling.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5D4FA5-E8BD-4F1F-A5D3-9B5AD624A763}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,22 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Stuff</t>
+  </si>
+  <si>
+    <t>May have done a bad design change, due to wanting to change values within movement modifiers during runtime such as gravityMagnitude, groundPullMagnitude, forceDrag, movementSpeed, jumpForce, etc…while keeping the movement modifier objects as POCO's without the SerializeField attributes, and the class itself not being serializable would mean that the constructor wouldn't get called automatically each time in the editor, to achieve this the values were delegated over to the corresponding MonoBehaviours and are passed in for the .Tick methods
+But this means that data builders can't work for them, and that they'll have to be passed as parameters each time. Perhaps this is okay with the current way it's set up but it doesn't sound exactly great
+The methods should have parameters that affect them, but they should function as lone objects as well, and this might require modification which in turn breaks the open closed principle as well
+Perhaps change this but keep the classes as POCO? But then the values would lose the ability to be changed during runtime in the inspector...?</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +64,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +348,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="80.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>